<commit_message>
maquina de estados terminada
</commit_message>
<xml_diff>
--- a/use-cases/use-case-selecionar-receita.xlsx
+++ b/use-cases/use-case-selecionar-receita.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\3A2S\LI4\projeto-li4\use-cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB094ED9-27E8-434E-9E80-4984D6466F78}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{053DCA31-5EE7-4459-8652-55030557F03D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4920" xr2:uid="{C7A0A64F-69DF-CB43-BB66-CA0002FD1B4D}"/>
   </bookViews>
@@ -716,15 +716,15 @@
   <dimension ref="B1:D27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="C4" sqref="C4:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.75" customWidth="1"/>
     <col min="2" max="2" width="25.75" customWidth="1"/>
-    <col min="3" max="3" width="50" customWidth="1"/>
-    <col min="4" max="4" width="50.75" customWidth="1"/>
+    <col min="3" max="3" width="50.875" customWidth="1"/>
+    <col min="4" max="4" width="52" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
falta acabar diagrama de classes
</commit_message>
<xml_diff>
--- a/use-cases/use-case-selecionar-receita.xlsx
+++ b/use-cases/use-case-selecionar-receita.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ricardopetronilho/Desktop/projeto-li4/use-cases/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\3A2S\LI4\projeto-li4\use-cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{235D36D8-456E-AE44-BBFD-E84BA5EA2886}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB0BB70C-F57A-4B1A-9320-B1B425C64ECF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="19540" xr2:uid="{C7A0A64F-69DF-CB43-BB66-CA0002FD1B4D}"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="38400" windowHeight="19545" xr2:uid="{C7A0A64F-69DF-CB43-BB66-CA0002FD1B4D}"/>
   </bookViews>
   <sheets>
     <sheet name="Realizar Receita (Ingredientes)" sheetId="1" r:id="rId1"/>
@@ -58,9 +58,6 @@
     <t>Ter Pesquisado Receita</t>
   </si>
   <si>
-    <t>Selecionar Receita (Ingredientes e SuperMercado)</t>
-  </si>
-  <si>
     <t>1. «include» Interpretar Comando de Voz</t>
   </si>
   <si>
@@ -127,9 +124,6 @@
     <t>Exceção 1</t>
   </si>
   <si>
-    <t>Exceção 3</t>
-  </si>
-  <si>
     <t>(passo 3 ou 3.4)</t>
   </si>
   <si>
@@ -140,6 +134,12 @@
   </si>
   <si>
     <t>Cliente</t>
+  </si>
+  <si>
+    <t>Selecionar Receita</t>
+  </si>
+  <si>
+    <t>Exceção 2</t>
   </si>
 </sst>
 </file>
@@ -405,7 +405,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -703,38 +703,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1247600E-1397-C742-A058-B663B513FA0A}">
   <dimension ref="B1:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.6640625" customWidth="1"/>
-    <col min="2" max="2" width="25.6640625" customWidth="1"/>
-    <col min="3" max="3" width="50.83203125" customWidth="1"/>
+    <col min="1" max="1" width="7.625" customWidth="1"/>
+    <col min="2" max="2" width="25.625" customWidth="1"/>
+    <col min="3" max="3" width="50.875" customWidth="1"/>
     <col min="4" max="4" width="52" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="7" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="D2" s="16"/>
     </row>
-    <row r="3" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="7" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D3" s="16"/>
     </row>
-    <row r="4" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="7" t="s">
         <v>5</v>
       </c>
@@ -743,7 +743,7 @@
       </c>
       <c r="D4" s="16"/>
     </row>
-    <row r="5" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B5" s="7" t="s">
         <v>6</v>
       </c>
@@ -752,7 +752,7 @@
       </c>
       <c r="D5" s="16"/>
     </row>
-    <row r="6" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="17" t="s">
         <v>2</v>
       </c>
@@ -763,148 +763,148 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:4" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:4" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="18"/>
       <c r="C7" s="5"/>
       <c r="D7" s="11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="2:4" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" s="18"/>
       <c r="C8" s="5"/>
       <c r="D8" s="11" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="2:4" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B9" s="18"/>
       <c r="C9" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D9" s="11"/>
     </row>
-    <row r="10" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" s="18"/>
       <c r="C10" s="5"/>
       <c r="D10" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B11" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="11" spans="2:4" ht="19" x14ac:dyDescent="0.25">
-      <c r="B11" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>15</v>
-      </c>
       <c r="D11" s="2"/>
     </row>
-    <row r="12" spans="2:4" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:4" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C12" s="5"/>
       <c r="D12" s="11" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="2:4" ht="19" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B13" s="9"/>
       <c r="C13" s="5"/>
       <c r="D13" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="14" spans="2:4" ht="19" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B14" s="9"/>
       <c r="C14" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B15" s="10"/>
       <c r="C15" s="6"/>
       <c r="D15" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="16" spans="2:4" ht="19" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B16" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D16" s="2"/>
     </row>
-    <row r="17" spans="2:4" ht="19" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B17" s="9" t="s">
         <v>8</v>
       </c>
       <c r="C17" s="5"/>
       <c r="D17" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B18" s="10" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C18" s="6"/>
       <c r="D18" s="3"/>
     </row>
-    <row r="19" spans="2:4" ht="19" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B19" s="8" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D19" s="2"/>
     </row>
-    <row r="20" spans="2:4" ht="19" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B20" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C20" s="5"/>
       <c r="D20" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4" ht="22" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B21" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C21" s="6"/>
       <c r="D21" s="3"/>
     </row>
-    <row r="22" spans="2:4" ht="19" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B22" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C22" s="4"/>
       <c r="D22" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="23" spans="2:4" ht="19" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B23" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D23" s="1"/>
+    </row>
+    <row r="24" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B24" s="10" t="s">
         <v>20</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D23" s="1"/>
-    </row>
-    <row r="24" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="10" t="s">
-        <v>21</v>
       </c>
       <c r="C24" s="6"/>
       <c r="D24" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>